<commit_message>
corrected a few errors in voting and simulate
</commit_message>
<xml_diff>
--- a/allt-thyskaland/matlab/table1.xlsx
+++ b/allt-thyskaland/matlab/table1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2568" uniqueCount="2568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2616" uniqueCount="2616">
   <si>
     <t>Row</t>
   </si>
@@ -92,6 +92,150 @@
   </si>
   <si>
     <t>CDU/CSU</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
   <si>
     <t>Row</t>
@@ -8137,33 +8281,33 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>2544</v>
+        <v>2592</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2561</v>
+        <v>2609</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>2562</v>
+        <v>2610</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>2563</v>
+        <v>2611</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2564</v>
+        <v>2612</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>2565</v>
+        <v>2613</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>2566</v>
+        <v>2614</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>2567</v>
+        <v>2615</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" s="0" t="s">
-        <v>2545</v>
+        <v>2593</v>
       </c>
       <c r="B2" s="2">
         <v>27.621156199911582</v>
@@ -8189,7 +8333,7 @@
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" s="0" t="s">
-        <v>2546</v>
+        <v>2594</v>
       </c>
       <c r="B3" s="2">
         <v>28.53361287910791</v>
@@ -8215,7 +8359,7 @@
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" s="0" t="s">
-        <v>2547</v>
+        <v>2595</v>
       </c>
       <c r="B4" s="2">
         <v>31.21299676230467</v>
@@ -8241,7 +8385,7 @@
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" s="0" t="s">
-        <v>2548</v>
+        <v>2596</v>
       </c>
       <c r="B5" s="2">
         <v>31.270325747781641</v>
@@ -8267,7 +8411,7 @@
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" s="0" t="s">
-        <v>2549</v>
+        <v>2597</v>
       </c>
       <c r="B6" s="2">
         <v>28.990210999389404</v>
@@ -8293,7 +8437,7 @@
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" s="0" t="s">
-        <v>2550</v>
+        <v>2598</v>
       </c>
       <c r="B7" s="2">
         <v>26.640347037971576</v>
@@ -8319,7 +8463,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" s="0" t="s">
-        <v>2551</v>
+        <v>2599</v>
       </c>
       <c r="B8" s="2">
         <v>27.005036768309242</v>
@@ -8345,7 +8489,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" s="0" t="s">
-        <v>2552</v>
+        <v>2600</v>
       </c>
       <c r="B9" s="2">
         <v>19.535587416781819</v>
@@ -8371,7 +8515,7 @@
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" s="0" t="s">
-        <v>2553</v>
+        <v>2601</v>
       </c>
       <c r="B10" s="2">
         <v>17.747760060036761</v>
@@ -8397,7 +8541,7 @@
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" s="0" t="s">
-        <v>2554</v>
+        <v>2602</v>
       </c>
       <c r="B11" s="2">
         <v>31.816588627103016</v>
@@ -8423,7 +8567,7 @@
     </row>
     <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" s="0" t="s">
-        <v>2555</v>
+        <v>2603</v>
       </c>
       <c r="B12" s="2">
         <v>21.969761225068776</v>
@@ -8449,7 +8593,7 @@
     </row>
     <row r="13" x14ac:dyDescent="0.2">
       <c r="A13" s="0" t="s">
-        <v>2556</v>
+        <v>2604</v>
       </c>
       <c r="B13" s="2">
         <v>23.383848067450923</v>
@@ -8475,7 +8619,7 @@
     </row>
     <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" s="0" t="s">
-        <v>2557</v>
+        <v>2605</v>
       </c>
       <c r="B14" s="2">
         <v>20.651777405316285</v>
@@ -8501,7 +8645,7 @@
     </row>
     <row r="15" x14ac:dyDescent="0.2">
       <c r="A15" s="0" t="s">
-        <v>2558</v>
+        <v>2606</v>
       </c>
       <c r="B15" s="2">
         <v>14.806675290256917</v>
@@ -8527,7 +8671,7 @@
     </row>
     <row r="16" x14ac:dyDescent="0.2">
       <c r="A16" s="0" t="s">
-        <v>2559</v>
+        <v>2607</v>
       </c>
       <c r="B16" s="2">
         <v>19.592636772135283</v>
@@ -8553,7 +8697,7 @@
     </row>
     <row r="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>2560</v>
+        <v>2608</v>
       </c>
       <c r="B17" s="6">
         <v>17.594084960104851</v>

</xml_diff>

<commit_message>
laga danska villu (Danskt_allt_Sim.json)
</commit_message>
<xml_diff>
--- a/allt-thyskaland/matlab/table1.xlsx
+++ b/allt-thyskaland/matlab/table1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5700" uniqueCount="5700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5820" uniqueCount="5820">
   <si>
     <t>Row</t>
   </si>
@@ -16667,6 +16667,366 @@
   </si>
   <si>
     <t>Saarland</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
   </si>
   <si>
     <t>SPD</t>
@@ -17534,28 +17894,28 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>5676</v>
+        <v>5796</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5693</v>
+        <v>5813</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5694</v>
+        <v>5814</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>5695</v>
+        <v>5815</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>5696</v>
+        <v>5816</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>5697</v>
+        <v>5817</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>5698</v>
+        <v>5818</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>5699</v>
+        <v>5819</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>5003</v>
@@ -17563,7 +17923,7 @@
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" s="0" t="s">
-        <v>5677</v>
+        <v>5797</v>
       </c>
       <c r="B2" s="2">
         <v>27.621156199911582</v>
@@ -17592,7 +17952,7 @@
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" s="0" t="s">
-        <v>5678</v>
+        <v>5798</v>
       </c>
       <c r="B3" s="2">
         <v>28.53361287910791</v>
@@ -17621,7 +17981,7 @@
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" s="0" t="s">
-        <v>5679</v>
+        <v>5799</v>
       </c>
       <c r="B4" s="2">
         <v>31.21299676230467</v>
@@ -17650,7 +18010,7 @@
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" s="0" t="s">
-        <v>5680</v>
+        <v>5800</v>
       </c>
       <c r="B5" s="2">
         <v>31.270325747781641</v>
@@ -17679,7 +18039,7 @@
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" s="0" t="s">
-        <v>5681</v>
+        <v>5801</v>
       </c>
       <c r="B6" s="2">
         <v>28.990210999389404</v>
@@ -17708,7 +18068,7 @@
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" s="0" t="s">
-        <v>5682</v>
+        <v>5802</v>
       </c>
       <c r="B7" s="2">
         <v>26.640347037971576</v>
@@ -17737,7 +18097,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" s="0" t="s">
-        <v>5683</v>
+        <v>5803</v>
       </c>
       <c r="B8" s="2">
         <v>27.005036768309242</v>
@@ -17766,7 +18126,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" s="0" t="s">
-        <v>5684</v>
+        <v>5804</v>
       </c>
       <c r="B9" s="2">
         <v>19.535587416781819</v>
@@ -17795,7 +18155,7 @@
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" s="0" t="s">
-        <v>5685</v>
+        <v>5805</v>
       </c>
       <c r="B10" s="2">
         <v>17.747760060036761</v>
@@ -17824,7 +18184,7 @@
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" s="0" t="s">
-        <v>5686</v>
+        <v>5806</v>
       </c>
       <c r="B11" s="2">
         <v>31.816588627103016</v>
@@ -17853,7 +18213,7 @@
     </row>
     <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" s="0" t="s">
-        <v>5687</v>
+        <v>5807</v>
       </c>
       <c r="B12" s="2">
         <v>21.969761225068776</v>
@@ -17882,7 +18242,7 @@
     </row>
     <row r="13" x14ac:dyDescent="0.2">
       <c r="A13" s="0" t="s">
-        <v>5688</v>
+        <v>5808</v>
       </c>
       <c r="B13" s="2">
         <v>20.651777405316285</v>
@@ -17911,7 +18271,7 @@
     </row>
     <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" s="0" t="s">
-        <v>5689</v>
+        <v>5809</v>
       </c>
       <c r="B14" s="2">
         <v>23.383848067450923</v>
@@ -17940,7 +18300,7 @@
     </row>
     <row r="15" x14ac:dyDescent="0.2">
       <c r="A15" s="0" t="s">
-        <v>5690</v>
+        <v>5810</v>
       </c>
       <c r="B15" s="2">
         <v>19.592636772135283</v>
@@ -17969,7 +18329,7 @@
     </row>
     <row r="16" x14ac:dyDescent="0.2">
       <c r="A16" s="0" t="s">
-        <v>5691</v>
+        <v>5811</v>
       </c>
       <c r="B16" s="2">
         <v>17.594084960104851</v>
@@ -17998,7 +18358,7 @@
     </row>
     <row r="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>5692</v>
+        <v>5812</v>
       </c>
       <c r="B17" s="6">
         <v>14.806675290256917</v>

</xml_diff>

<commit_message>
restore after git corruption
</commit_message>
<xml_diff>
--- a/allt-thyskaland/matlab/table1.xlsx
+++ b/allt-thyskaland/matlab/table1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5820" uniqueCount="5820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6444" uniqueCount="6444">
   <si>
     <t>Row</t>
   </si>
@@ -16667,6 +16667,1878 @@
   </si>
   <si>
     <t>Saarland</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
+  </si>
+  <si>
+    <t>SPD</t>
+  </si>
+  <si>
+    <t>FDP</t>
+  </si>
+  <si>
+    <t>Grüne</t>
+  </si>
+  <si>
+    <t>Linke</t>
+  </si>
+  <si>
+    <t>AfD</t>
+  </si>
+  <si>
+    <t>CDU</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>Schleswig-Holstein</t>
+  </si>
+  <si>
+    <t>Hamburg</t>
+  </si>
+  <si>
+    <t>Niedersachsen</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>Nordrhein-Westfalen</t>
+  </si>
+  <si>
+    <t>Hessen</t>
+  </si>
+  <si>
+    <t>Rheinland-Pfalz</t>
+  </si>
+  <si>
+    <t>Baden-Württemberg</t>
+  </si>
+  <si>
+    <t>Bayern</t>
+  </si>
+  <si>
+    <t>Saarland</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>Mecklenburg-Vorpommern</t>
+  </si>
+  <si>
+    <t>Brandenburg</t>
+  </si>
+  <si>
+    <t>Sachsen-Anhalt</t>
+  </si>
+  <si>
+    <t>Thüringen</t>
+  </si>
+  <si>
+    <t>Sachsen</t>
   </si>
   <si>
     <t>SPD</t>
@@ -17894,28 +19766,28 @@
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>5796</v>
+        <v>6420</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5813</v>
+        <v>6437</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>5814</v>
+        <v>6438</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>5815</v>
+        <v>6439</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>5816</v>
+        <v>6440</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>5817</v>
+        <v>6441</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>5818</v>
+        <v>6442</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>5819</v>
+        <v>6443</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>5003</v>
@@ -17923,7 +19795,7 @@
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" s="0" t="s">
-        <v>5797</v>
+        <v>6421</v>
       </c>
       <c r="B2" s="2">
         <v>27.621156199911582</v>
@@ -17952,7 +19824,7 @@
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" s="0" t="s">
-        <v>5798</v>
+        <v>6422</v>
       </c>
       <c r="B3" s="2">
         <v>28.53361287910791</v>
@@ -17981,7 +19853,7 @@
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" s="0" t="s">
-        <v>5799</v>
+        <v>6423</v>
       </c>
       <c r="B4" s="2">
         <v>31.21299676230467</v>
@@ -18010,7 +19882,7 @@
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" s="0" t="s">
-        <v>5800</v>
+        <v>6424</v>
       </c>
       <c r="B5" s="2">
         <v>31.270325747781641</v>
@@ -18039,7 +19911,7 @@
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" s="0" t="s">
-        <v>5801</v>
+        <v>6425</v>
       </c>
       <c r="B6" s="2">
         <v>28.990210999389404</v>
@@ -18068,7 +19940,7 @@
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" s="0" t="s">
-        <v>5802</v>
+        <v>6426</v>
       </c>
       <c r="B7" s="2">
         <v>26.640347037971576</v>
@@ -18097,7 +19969,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" s="0" t="s">
-        <v>5803</v>
+        <v>6427</v>
       </c>
       <c r="B8" s="2">
         <v>27.005036768309242</v>
@@ -18126,7 +19998,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" s="0" t="s">
-        <v>5804</v>
+        <v>6428</v>
       </c>
       <c r="B9" s="2">
         <v>19.535587416781819</v>
@@ -18155,7 +20027,7 @@
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" s="0" t="s">
-        <v>5805</v>
+        <v>6429</v>
       </c>
       <c r="B10" s="2">
         <v>17.747760060036761</v>
@@ -18184,7 +20056,7 @@
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" s="0" t="s">
-        <v>5806</v>
+        <v>6430</v>
       </c>
       <c r="B11" s="2">
         <v>31.816588627103016</v>
@@ -18213,7 +20085,7 @@
     </row>
     <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" s="0" t="s">
-        <v>5807</v>
+        <v>6431</v>
       </c>
       <c r="B12" s="2">
         <v>21.969761225068776</v>
@@ -18242,7 +20114,7 @@
     </row>
     <row r="13" x14ac:dyDescent="0.2">
       <c r="A13" s="0" t="s">
-        <v>5808</v>
+        <v>6432</v>
       </c>
       <c r="B13" s="2">
         <v>20.651777405316285</v>
@@ -18271,7 +20143,7 @@
     </row>
     <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" s="0" t="s">
-        <v>5809</v>
+        <v>6433</v>
       </c>
       <c r="B14" s="2">
         <v>23.383848067450923</v>
@@ -18300,7 +20172,7 @@
     </row>
     <row r="15" x14ac:dyDescent="0.2">
       <c r="A15" s="0" t="s">
-        <v>5810</v>
+        <v>6434</v>
       </c>
       <c r="B15" s="2">
         <v>19.592636772135283</v>
@@ -18329,7 +20201,7 @@
     </row>
     <row r="16" x14ac:dyDescent="0.2">
       <c r="A16" s="0" t="s">
-        <v>5811</v>
+        <v>6435</v>
       </c>
       <c r="B16" s="2">
         <v>17.594084960104851</v>
@@ -18358,7 +20230,7 @@
     </row>
     <row r="17" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>5812</v>
+        <v>6436</v>
       </c>
       <c r="B17" s="6">
         <v>14.806675290256917</v>

</xml_diff>